<commit_message>
adjust sample_transformer for new g3t_etl.transformer
</commit_message>
<xml_diff>
--- a/tests/fixtures/sample_data_dictionary.xlsx
+++ b/tests/fixtures/sample_data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walsbr/aced/g3t_etl/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50ABF09F-5466-EA4D-A35E-9885A9F8D372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E916DE-9CE5-0D46-84BF-6DD1AC47FEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17260" yWindow="-19280" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fhir_mapping" sheetId="4" r:id="rId1"/>
@@ -692,9 +692,6 @@
     <t>observation_subject</t>
   </si>
   <si>
-    <t>Patient, Specimen, Condition</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
@@ -837,6 +834,9 @@
   </si>
   <si>
     <t>Procedure</t>
+  </si>
+  <si>
+    <t>Patient.identifier</t>
   </si>
 </sst>
 </file>
@@ -1783,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF306E1-1D33-D74E-9073-4A3E9E8DA547}">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1834,13 +1834,13 @@
         <v>165</v>
       </c>
       <c r="K1" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="L1" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="M1" s="36" t="s">
         <v>169</v>
-      </c>
-      <c r="M1" s="36" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="32"/>
@@ -1880,14 +1880,14 @@
         <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="32"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -1913,13 +1913,13 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L4" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -1934,29 +1934,29 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="G5" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="H5" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>187</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -1971,29 +1971,29 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F6" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="G6" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="H6" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>197</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K6" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
@@ -2008,14 +2008,14 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="32"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -2026,36 +2026,36 @@
         <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F8" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="G8" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="H8" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>197</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K8" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -2070,23 +2070,23 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="32"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K9" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L9" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="M9" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.15">
@@ -2101,20 +2101,20 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G10" s="33">
         <v>372278000</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -2132,29 +2132,29 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G11" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>199</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.15">
@@ -2169,14 +2169,14 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="32"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -2194,29 +2194,29 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G13" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>193</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K13" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.15">
@@ -2231,14 +2231,14 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="32"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
@@ -2256,14 +2256,14 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="32"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
@@ -2281,14 +2281,14 @@
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="32"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
@@ -2306,14 +2306,14 @@
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="32"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
@@ -2333,20 +2333,20 @@
         <v>45413</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G18" s="32">
         <v>273575009</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
@@ -2366,20 +2366,20 @@
         <v>45413</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G19" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>201</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
@@ -2399,14 +2399,14 @@
         <v>45413</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="32"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
@@ -2424,29 +2424,29 @@
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G21" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K21" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -2461,23 +2461,23 @@
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="32"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K22" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -2492,23 +2492,23 @@
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="32"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K23" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.15">
@@ -2525,14 +2525,14 @@
         <v>14</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="32"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -2550,20 +2550,20 @@
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G25" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
@@ -2581,23 +2581,23 @@
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="32"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K26" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -2612,23 +2612,23 @@
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="32"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K27" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.15">
@@ -2643,20 +2643,20 @@
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G28" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>208</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -2674,29 +2674,29 @@
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H29" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K29" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.15">
@@ -2711,20 +2711,20 @@
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F30" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G30" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="H30" s="32" t="s">
         <v>211</v>
-      </c>
-      <c r="H30" s="32" t="s">
-        <v>212</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -2742,14 +2742,14 @@
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="32"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
@@ -2767,14 +2767,14 @@
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="32"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -2792,23 +2792,23 @@
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="32"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K33" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L33" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L33" s="28" t="s">
+      <c r="M33" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M33" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -2823,23 +2823,23 @@
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="32"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K34" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L34" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L34" s="28" t="s">
+      <c r="M34" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M34" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -2854,23 +2854,23 @@
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="32"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K35" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L35" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L35" s="28" t="s">
+      <c r="M35" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M35" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -2885,23 +2885,23 @@
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="32"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K36" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L36" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L36" s="28" t="s">
+      <c r="M36" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M36" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.15">
@@ -2916,14 +2916,14 @@
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="32"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
       <c r="J37" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -2941,14 +2941,14 @@
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="32"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
@@ -2966,14 +2966,14 @@
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="32"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
@@ -2991,23 +2991,23 @@
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="32"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K40" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L40" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L40" s="28" t="s">
+      <c r="M40" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M40" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -3022,23 +3022,23 @@
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="32"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K41" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L41" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L41" s="28" t="s">
+      <c r="M41" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M41" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -3053,23 +3053,23 @@
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="32"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K42" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L42" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L42" s="28" t="s">
+      <c r="M42" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M42" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -3084,23 +3084,23 @@
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="32"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K43" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L43" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L43" s="28" t="s">
+      <c r="M43" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M43" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -3115,23 +3115,23 @@
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="32"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K44" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L44" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L44" s="28" t="s">
+      <c r="M44" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M44" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -3146,23 +3146,23 @@
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="32"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K45" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L45" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L45" s="28" t="s">
+      <c r="M45" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M45" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -3177,23 +3177,23 @@
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="32"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K46" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L46" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L46" s="28" t="s">
+      <c r="M46" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M46" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -3208,23 +3208,23 @@
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="32"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K47" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L47" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L47" s="28" t="s">
+      <c r="M47" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M47" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -3239,23 +3239,23 @@
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="32"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K48" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L48" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L48" s="28" t="s">
+      <c r="M48" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M48" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -3270,23 +3270,23 @@
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="32"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K49" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="L49" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="L49" s="28" t="s">
+      <c r="M49" s="28" t="s">
         <v>172</v>
-      </c>
-      <c r="M49" s="28" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.15">
@@ -3303,20 +3303,20 @@
         <v>134</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F50" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G50" s="32">
         <v>372278000</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I50" s="4"/>
       <c r="J50" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
@@ -3336,20 +3336,20 @@
         <v>134</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F51" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G51" s="32">
         <v>372278000</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I51" s="4"/>
       <c r="J51" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
@@ -3369,14 +3369,14 @@
         <v>134</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="32"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -4764,21 +4764,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001D56C3C813D16D47A25D8147D4BCAE76" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="654604e9b9c1a560e8a2f89a1fff65b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d8356f0e-69ae-4183-add8-26fde198cf5f" xmlns:ns3="82bababd-4ad0-4e81-b6b3-ef3af3f58d2c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5bf9c17f493d9ff9480a8b8065d04d65" ns2:_="" ns3:_="">
     <xsd:import namespace="d8356f0e-69ae-4183-add8-26fde198cf5f"/>
@@ -4979,24 +4964,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BA9FDD3-FFD6-4FE9-AFCD-4D29890A0C2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDEA044C-0ACA-4416-A3F7-BFB93CA4148D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C779103-5E7D-471C-B69F-43DD7CD417F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5013,4 +4996,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDEA044C-0ACA-4416-A3F7-BFB93CA4148D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BA9FDD3-FFD6-4FE9-AFCD-4D29890A0C2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>